<commit_message>
Testing Egg Timer Counter
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData1.xlsx
+++ b/src/test/resources/testData/TestData1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A1D6BA-D8E0-4BE1-A074-9EA322C0EF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB85606-079A-4065-AD55-1234DFDFB7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>endOfTestData</t>
   </si>
@@ -58,10 +58,16 @@
     <t>elementName</t>
   </si>
   <si>
-    <t>xyz@yahoo.comUsr</t>
-  </si>
-  <si>
-    <t>abc@123$</t>
+    <t>timerCount</t>
+  </si>
+  <si>
+    <t>testTimerCounterValue</t>
+  </si>
+  <si>
+    <t>myplayer@yahoo.comUsr</t>
+  </si>
+  <si>
+    <t>Rajuway@123$</t>
   </si>
 </sst>
 </file>
@@ -103,11 +109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,11 +425,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -443,11 +452,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -471,13 +480,12 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3"/>
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -530,15 +538,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>25</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{AF85A300-4499-40C9-8457-9E202CED3D34}"/>
-    <hyperlink ref="A7" r:id="rId2" xr:uid="{BC93AC6B-2350-458D-AEDA-CA4C914609C4}"/>
-    <hyperlink ref="A11" r:id="rId3" xr:uid="{0A363BBD-5EE4-4CC8-8C42-A1AA40A414BE}"/>
-    <hyperlink ref="B7" r:id="rId4" xr:uid="{C3FAA826-2F37-450D-94B1-25F760EE8DD9}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{E9C666FD-3450-46D4-ACB5-F828CF7BE17A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>